<commit_message>
refactor: to reduce the used gas #11
- Use revert instead of require
- Replacing Modifiers with Functions
</commit_message>
<xml_diff>
--- a/outputFile/log-used-gas.xlsx
+++ b/outputFile/log-used-gas.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F58"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -536,10 +536,10 @@
         <v/>
       </c>
       <c r="E7" t="str">
-        <v>89669</v>
+        <v>89648</v>
       </c>
       <c r="F7" t="str">
-        <v>0.00089669</v>
+        <v>0.00089648</v>
       </c>
     </row>
     <row r="8">
@@ -564,62 +564,62 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>Layer2Manager</v>
+        <v>L2Registry</v>
       </c>
       <c r="B9" t="str">
-        <v>registerLayer2Candidate</v>
+        <v>registerSystemConfigByManager</v>
       </c>
       <c r="C9" t="str">
         <v/>
       </c>
       <c r="D9" t="str">
-        <v>using registerLayer2Candidate function</v>
+        <v xml:space="preserve">Thanos SystemConfig </v>
       </c>
       <c r="E9" t="str">
-        <v>4862534</v>
+        <v>98997</v>
       </c>
       <c r="F9" t="str">
-        <v>0.04862534</v>
+        <v>0.00098997</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>SeigManagerV1_3</v>
+        <v>Layer2Manager</v>
       </c>
       <c r="B10" t="str">
-        <v>setLayer2StartBlock</v>
+        <v>registerLayer2Candidate</v>
       </c>
       <c r="C10" t="str">
         <v/>
       </c>
       <c r="D10" t="str">
-        <v/>
+        <v>using registerLayer2Candidate function</v>
       </c>
       <c r="E10" t="str">
-        <v>56913</v>
+        <v>4862471</v>
       </c>
       <c r="F10" t="str">
-        <v>0.00056913</v>
+        <v>0.04862471</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>DepositManager</v>
+        <v>SeigManagerV1_3</v>
       </c>
       <c r="B11" t="str">
-        <v>approveAndCall</v>
+        <v>setLayer2StartBlock</v>
       </c>
       <c r="C11" t="str">
         <v/>
       </c>
       <c r="D11" t="str">
-        <v>deposit TON to Titan Candidate</v>
+        <v/>
       </c>
       <c r="E11" t="str">
-        <v>374814</v>
+        <v>56913</v>
       </c>
       <c r="F11" t="str">
-        <v>0.00374814</v>
+        <v>0.00056913</v>
       </c>
     </row>
     <row r="12">
@@ -627,19 +627,19 @@
         <v>DepositManager</v>
       </c>
       <c r="B12" t="str">
-        <v>deposit(address,uint256)</v>
+        <v>approveAndCall</v>
       </c>
       <c r="C12" t="str">
         <v/>
       </c>
       <c r="D12" t="str">
-        <v>deposit WTON to Titan Candidate</v>
+        <v>deposit TON to Titan Candidate</v>
       </c>
       <c r="E12" t="str">
-        <v>303991</v>
+        <v>374814</v>
       </c>
       <c r="F12" t="str">
-        <v>0.00303991</v>
+        <v>0.00374814</v>
       </c>
     </row>
     <row r="13">
@@ -647,7 +647,7 @@
         <v>DepositManager</v>
       </c>
       <c r="B13" t="str">
-        <v>deposit(address,address,uint256)</v>
+        <v>deposit(address,uint256)</v>
       </c>
       <c r="C13" t="str">
         <v/>
@@ -656,30 +656,30 @@
         <v>deposit WTON to Titan Candidate</v>
       </c>
       <c r="E13" t="str">
-        <v>254169</v>
+        <v>303991</v>
       </c>
       <c r="F13" t="str">
-        <v>0.00254169</v>
+        <v>0.00303991</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>SeigManagerV1_3</v>
+        <v>DepositManager</v>
       </c>
       <c r="B14" t="str">
-        <v>updateSeigniorageLayer(layerAddress)</v>
+        <v>deposit(address,address,uint256)</v>
       </c>
       <c r="C14" t="str">
         <v/>
       </c>
       <c r="D14" t="str">
-        <v>the first updateSeigniorage : no give seigniorage to l2</v>
+        <v>deposit WTON to Titan Candidate</v>
       </c>
       <c r="E14" t="str">
-        <v>429881</v>
+        <v>254169</v>
       </c>
       <c r="F14" t="str">
-        <v>0.00429881</v>
+        <v>0.00254169</v>
       </c>
     </row>
     <row r="15">
@@ -693,13 +693,13 @@
         <v/>
       </c>
       <c r="D15" t="str">
-        <v>the second updateSeigniorage : not operator</v>
+        <v>the first updateSeigniorage : no give seigniorage to l2</v>
       </c>
       <c r="E15" t="str">
-        <v>437728</v>
+        <v>429640</v>
       </c>
       <c r="F15" t="str">
-        <v>0.00437728</v>
+        <v>0.0042964</v>
       </c>
     </row>
     <row r="16">
@@ -707,19 +707,19 @@
         <v>SeigManagerV1_3</v>
       </c>
       <c r="B16" t="str">
-        <v>updateSeigniorage(1)</v>
+        <v>updateSeigniorageLayer(layerAddress)</v>
       </c>
       <c r="C16" t="str">
         <v/>
       </c>
       <c r="D16" t="str">
-        <v>the third updateSeigniorage of operator with claiming</v>
+        <v>the second updateSeigniorage : not operator</v>
       </c>
       <c r="E16" t="str">
-        <v>481034</v>
+        <v>437487</v>
       </c>
       <c r="F16" t="str">
-        <v>0.00481034</v>
+        <v>0.00437487</v>
       </c>
     </row>
     <row r="17">
@@ -727,39 +727,39 @@
         <v>SeigManagerV1_3</v>
       </c>
       <c r="B17" t="str">
-        <v>updateSeigniorage(2)</v>
+        <v>updateSeigniorage(1)</v>
       </c>
       <c r="C17" t="str">
         <v/>
       </c>
       <c r="D17" t="str">
-        <v xml:space="preserve">the forth updateSeigniorage of operator with staking </v>
+        <v>the third updateSeigniorage of operator with claiming</v>
       </c>
       <c r="E17" t="str">
-        <v>588504</v>
+        <v>480766</v>
       </c>
       <c r="F17" t="str">
-        <v>0.00588504</v>
+        <v>0.00480766</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>DepositManager</v>
+        <v>SeigManagerV1_3</v>
       </c>
       <c r="B18" t="str">
-        <v>requestWithdrawal</v>
+        <v>updateSeigniorage(2)</v>
       </c>
       <c r="C18" t="str">
         <v/>
       </c>
       <c r="D18" t="str">
-        <v/>
+        <v xml:space="preserve">the forth updateSeigniorage of operator with staking </v>
       </c>
       <c r="E18" t="str">
-        <v>340683</v>
+        <v>588263</v>
       </c>
       <c r="F18" t="str">
-        <v>0.00340683</v>
+        <v>0.00588263</v>
       </c>
     </row>
     <row r="19">
@@ -767,7 +767,7 @@
         <v>DepositManager</v>
       </c>
       <c r="B19" t="str">
-        <v>processRequest</v>
+        <v>requestWithdrawal</v>
       </c>
       <c r="C19" t="str">
         <v/>
@@ -776,10 +776,10 @@
         <v/>
       </c>
       <c r="E19" t="str">
-        <v>197362</v>
+        <v>341275</v>
       </c>
       <c r="F19" t="str">
-        <v>0.00197362</v>
+        <v>0.00341275</v>
       </c>
     </row>
     <row r="20">
@@ -787,19 +787,19 @@
         <v>DepositManager</v>
       </c>
       <c r="B20" t="str">
-        <v>approveAndCall</v>
+        <v>processRequest</v>
       </c>
       <c r="C20" t="str">
         <v/>
       </c>
       <c r="D20" t="str">
-        <v>deposit TON to DAOCandidate</v>
+        <v/>
       </c>
       <c r="E20" t="str">
-        <v>315110</v>
+        <v>197362</v>
       </c>
       <c r="F20" t="str">
-        <v>0.0031511</v>
+        <v>0.00197362</v>
       </c>
     </row>
     <row r="21">
@@ -816,10 +816,10 @@
         <v>deposit TON to DAOCandidate</v>
       </c>
       <c r="E21" t="str">
-        <v>356170</v>
+        <v>315110</v>
       </c>
       <c r="F21" t="str">
-        <v>0.0035617</v>
+        <v>0.0031511</v>
       </c>
     </row>
     <row r="22">
@@ -827,19 +827,19 @@
         <v>DepositManager</v>
       </c>
       <c r="B22" t="str">
-        <v>deposit(address,uint256)</v>
+        <v>approveAndCall</v>
       </c>
       <c r="C22" t="str">
         <v/>
       </c>
       <c r="D22" t="str">
-        <v>deposit WTON to DAOCandidate</v>
+        <v>deposit TON to DAOCandidate</v>
       </c>
       <c r="E22" t="str">
-        <v>249099</v>
+        <v>356170</v>
       </c>
       <c r="F22" t="str">
-        <v>0.00249099</v>
+        <v>0.0035617</v>
       </c>
     </row>
     <row r="23">
@@ -847,7 +847,7 @@
         <v>DepositManager</v>
       </c>
       <c r="B23" t="str">
-        <v>deposit(address,address,uint256)</v>
+        <v>deposit(address,uint256)</v>
       </c>
       <c r="C23" t="str">
         <v/>
@@ -856,50 +856,50 @@
         <v>deposit WTON to DAOCandidate</v>
       </c>
       <c r="E23" t="str">
-        <v>290666</v>
+        <v>249099</v>
       </c>
       <c r="F23" t="str">
-        <v>0.00290666</v>
+        <v>0.00249099</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>SeigManagerV1_3</v>
+        <v>DepositManager</v>
       </c>
       <c r="B24" t="str">
-        <v>updateSeigniorageLayer(layerAddress)</v>
+        <v>deposit(address,address,uint256)</v>
       </c>
       <c r="C24" t="str">
         <v/>
       </c>
       <c r="D24" t="str">
-        <v>updateSeigniorage to DAOCandidate</v>
+        <v>deposit WTON to DAOCandidate</v>
       </c>
       <c r="E24" t="str">
-        <v>348174</v>
+        <v>290666</v>
       </c>
       <c r="F24" t="str">
-        <v>0.00348174</v>
+        <v>0.00290666</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>DepositManager</v>
+        <v>SeigManagerV1_3</v>
       </c>
       <c r="B25" t="str">
-        <v>requestWithdrawal(address,uint256)</v>
+        <v>updateSeigniorageLayer(layerAddress)</v>
       </c>
       <c r="C25" t="str">
         <v/>
       </c>
       <c r="D25" t="str">
-        <v/>
+        <v>updateSeigniorage to DAOCandidate</v>
       </c>
       <c r="E25" t="str">
-        <v>278176</v>
+        <v>347933</v>
       </c>
       <c r="F25" t="str">
-        <v>0.00278176</v>
+        <v>0.00347933</v>
       </c>
     </row>
     <row r="26">
@@ -907,7 +907,7 @@
         <v>DepositManager</v>
       </c>
       <c r="B26" t="str">
-        <v>processRequests(address,uint256,bool)</v>
+        <v>requestWithdrawal(address,uint256)</v>
       </c>
       <c r="C26" t="str">
         <v/>
@@ -916,10 +916,10 @@
         <v/>
       </c>
       <c r="E26" t="str">
-        <v>145889</v>
+        <v>278176</v>
       </c>
       <c r="F26" t="str">
-        <v>0.00145889</v>
+        <v>0.00278176</v>
       </c>
     </row>
     <row r="27">
@@ -927,19 +927,19 @@
         <v>DepositManager</v>
       </c>
       <c r="B27" t="str">
-        <v>approveAndCall</v>
+        <v>processRequests(address,uint256,bool)</v>
       </c>
       <c r="C27" t="str">
         <v/>
       </c>
       <c r="D27" t="str">
-        <v>deposit TON to Titan Layer2 Candidate</v>
+        <v/>
       </c>
       <c r="E27" t="str">
-        <v>357714</v>
+        <v>145889</v>
       </c>
       <c r="F27" t="str">
-        <v>0.00357714</v>
+        <v>0.00145889</v>
       </c>
     </row>
     <row r="28">
@@ -953,13 +953,13 @@
         <v/>
       </c>
       <c r="D28" t="str">
-        <v>deposit TON to DAO Candidate</v>
+        <v>deposit TON to Titan Layer2 Candidate</v>
       </c>
       <c r="E28" t="str">
-        <v>322941</v>
+        <v>357714</v>
       </c>
       <c r="F28" t="str">
-        <v>0.00322941</v>
+        <v>0.00357714</v>
       </c>
     </row>
     <row r="29">
@@ -967,24 +967,604 @@
         <v>DepositManager</v>
       </c>
       <c r="B29" t="str">
+        <v>approveAndCall</v>
+      </c>
+      <c r="C29" t="str">
+        <v/>
+      </c>
+      <c r="D29" t="str">
+        <v>deposit TON to DAO Candidate</v>
+      </c>
+      <c r="E29" t="str">
+        <v>322941</v>
+      </c>
+      <c r="F29" t="str">
+        <v>0.00322941</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>DepositManager</v>
+      </c>
+      <c r="B30" t="str">
         <v>withdrawAndDepositL2</v>
       </c>
-      <c r="C29" t="str">
-        <v/>
-      </c>
-      <c r="D29" t="str">
-        <v/>
-      </c>
-      <c r="E29" t="str">
+      <c r="C30" t="str">
+        <v/>
+      </c>
+      <c r="D30" t="str">
+        <v/>
+      </c>
+      <c r="E30" t="str">
         <v>476145</v>
       </c>
-      <c r="F29" t="str">
+      <c r="F30" t="str">
         <v>0.00476145</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>L2Registry</v>
+      </c>
+      <c r="B31" t="str">
+        <v>rejectLayer2Candidate</v>
+      </c>
+      <c r="C31" t="str">
+        <v/>
+      </c>
+      <c r="D31" t="str">
+        <v>legacySystemConfig</v>
+      </c>
+      <c r="E31" t="str">
+        <v>115789</v>
+      </c>
+      <c r="F31" t="str">
+        <v>0.00115789</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>L2Registry</v>
+      </c>
+      <c r="B32" t="str">
+        <v>registerLayer2Candidate</v>
+      </c>
+      <c r="C32" t="str">
+        <v/>
+      </c>
+      <c r="D32" t="str">
+        <v>thanos SystemConfig</v>
+      </c>
+      <c r="E32" t="str">
+        <v>4823637</v>
+      </c>
+      <c r="F32" t="str">
+        <v>0.04823637</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>SeigManager</v>
+      </c>
+      <c r="B33" t="str">
+        <v>updateSeigniorageLayer</v>
+      </c>
+      <c r="C33" t="str">
+        <v/>
+      </c>
+      <c r="D33" t="str">
+        <v>titanLayerAddress</v>
+      </c>
+      <c r="E33" t="str">
+        <v>355902</v>
+      </c>
+      <c r="F33" t="str">
+        <v>0.00355902</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>titanLayerContract</v>
+      </c>
+      <c r="B34" t="str">
+        <v>updateSeigniorage</v>
+      </c>
+      <c r="C34" t="str">
+        <v/>
+      </c>
+      <c r="D34" t="str">
+        <v>with claim</v>
+      </c>
+      <c r="E34" t="str">
+        <v>355815</v>
+      </c>
+      <c r="F34" t="str">
+        <v>0.00355815</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>titanLayerContract</v>
+      </c>
+      <c r="B35" t="str">
+        <v>updateSeigniorage</v>
+      </c>
+      <c r="C35" t="str">
+        <v/>
+      </c>
+      <c r="D35" t="str">
+        <v>with staking</v>
+      </c>
+      <c r="E35" t="str">
+        <v>355815</v>
+      </c>
+      <c r="F35" t="str">
+        <v>0.00355815</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>DepositManager</v>
+      </c>
+      <c r="B36" t="str">
+        <v>deposit(address,uint256)</v>
+      </c>
+      <c r="C36" t="str">
+        <v/>
+      </c>
+      <c r="D36" t="str">
+        <v/>
+      </c>
+      <c r="E36" t="str">
+        <v>286891</v>
+      </c>
+      <c r="F36" t="str">
+        <v>0.00286891</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>SeigManager</v>
+      </c>
+      <c r="B37" t="str">
+        <v>updateSeigniorageLayer</v>
+      </c>
+      <c r="C37" t="str">
+        <v/>
+      </c>
+      <c r="D37" t="str">
+        <v>no give seigniorage to l2</v>
+      </c>
+      <c r="E37" t="str">
+        <v>435106</v>
+      </c>
+      <c r="F37" t="str">
+        <v>0.00435106</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>DepositManager</v>
+      </c>
+      <c r="B38" t="str">
+        <v>deposit(address,address,uint256)</v>
+      </c>
+      <c r="C38" t="str">
+        <v/>
+      </c>
+      <c r="D38" t="str">
+        <v/>
+      </c>
+      <c r="E38" t="str">
+        <v>254169</v>
+      </c>
+      <c r="F38" t="str">
+        <v>0.00254169</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>SeigManager</v>
+      </c>
+      <c r="B39" t="str">
+        <v>updateSeigniorageLayer</v>
+      </c>
+      <c r="C39" t="str">
+        <v/>
+      </c>
+      <c r="D39" t="str">
+        <v>give seigniorage to l2</v>
+      </c>
+      <c r="E39" t="str">
+        <v>408491</v>
+      </c>
+      <c r="F39" t="str">
+        <v>0.00408491</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>SeigManager</v>
+      </c>
+      <c r="B40" t="str">
+        <v>updateSeigniorageLayer</v>
+      </c>
+      <c r="C40" t="str">
+        <v/>
+      </c>
+      <c r="D40" t="str">
+        <v>not operator</v>
+      </c>
+      <c r="E40" t="str">
+        <v>408491</v>
+      </c>
+      <c r="F40" t="str">
+        <v>0.00408491</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>Layer2Contract</v>
+      </c>
+      <c r="B41" t="str">
+        <v>updateSeigniorage</v>
+      </c>
+      <c r="C41" t="str">
+        <v/>
+      </c>
+      <c r="D41" t="str">
+        <v>operator</v>
+      </c>
+      <c r="E41" t="str">
+        <v>485970</v>
+      </c>
+      <c r="F41" t="str">
+        <v>0.0048597</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>Layer2Contract</v>
+      </c>
+      <c r="B42" t="str">
+        <v>updateSeigniorage</v>
+      </c>
+      <c r="C42" t="str">
+        <v/>
+      </c>
+      <c r="D42" t="str">
+        <v>with operator's staking</v>
+      </c>
+      <c r="E42" t="str">
+        <v>593467</v>
+      </c>
+      <c r="F42" t="str">
+        <v>0.00593467</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>DepositManager</v>
+      </c>
+      <c r="B43" t="str">
+        <v>requestWithdrawal</v>
+      </c>
+      <c r="C43" t="str">
+        <v/>
+      </c>
+      <c r="D43" t="str">
+        <v/>
+      </c>
+      <c r="E43" t="str">
+        <v>341275</v>
+      </c>
+      <c r="F43" t="str">
+        <v>0.00341275</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>DepositManager</v>
+      </c>
+      <c r="B44" t="str">
+        <v>processRequest</v>
+      </c>
+      <c r="C44" t="str">
+        <v/>
+      </c>
+      <c r="D44" t="str">
+        <v/>
+      </c>
+      <c r="E44" t="str">
+        <v>180262</v>
+      </c>
+      <c r="F44" t="str">
+        <v>0.00180262</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>L2Registry</v>
+      </c>
+      <c r="B45" t="str">
+        <v>restoreLayer2Candidate</v>
+      </c>
+      <c r="C45" t="str">
+        <v/>
+      </c>
+      <c r="D45" t="str">
+        <v/>
+      </c>
+      <c r="E45" t="str">
+        <v>72294</v>
+      </c>
+      <c r="F45" t="str">
+        <v>0.00072294</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>SeigManager</v>
+      </c>
+      <c r="B46" t="str">
+        <v>updateSeigniorageLayer</v>
+      </c>
+      <c r="C46" t="str">
+        <v/>
+      </c>
+      <c r="D46" t="str">
+        <v/>
+      </c>
+      <c r="E46" t="str">
+        <v>425987</v>
+      </c>
+      <c r="F46" t="str">
+        <v>0.00425987</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>SeigManager</v>
+      </c>
+      <c r="B47" t="str">
+        <v>updateSeigniorageLayer</v>
+      </c>
+      <c r="C47" t="str">
+        <v/>
+      </c>
+      <c r="D47" t="str">
+        <v/>
+      </c>
+      <c r="E47" t="str">
+        <v>403287</v>
+      </c>
+      <c r="F47" t="str">
+        <v>0.00403287</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>SeigManager</v>
+      </c>
+      <c r="B48" t="str">
+        <v>updateSeigniorageLayer</v>
+      </c>
+      <c r="C48" t="str">
+        <v/>
+      </c>
+      <c r="D48" t="str">
+        <v/>
+      </c>
+      <c r="E48" t="str">
+        <v>403287</v>
+      </c>
+      <c r="F48" t="str">
+        <v>0.00403287</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>Layer2Contract</v>
+      </c>
+      <c r="B49" t="str">
+        <v>updateSeigniorage</v>
+      </c>
+      <c r="C49" t="str">
+        <v/>
+      </c>
+      <c r="D49" t="str">
+        <v>with operator's claim</v>
+      </c>
+      <c r="E49" t="str">
+        <v>463666</v>
+      </c>
+      <c r="F49" t="str">
+        <v>0.00463666</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>Layer2Contract</v>
+      </c>
+      <c r="B50" t="str">
+        <v>updateSeigniorage</v>
+      </c>
+      <c r="C50" t="str">
+        <v/>
+      </c>
+      <c r="D50" t="str">
+        <v>with operator's staking</v>
+      </c>
+      <c r="E50" t="str">
+        <v>567880</v>
+      </c>
+      <c r="F50" t="str">
+        <v>0.0056788</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>DepositManager</v>
+      </c>
+      <c r="B51" t="str">
+        <v>requestWithdrawal</v>
+      </c>
+      <c r="C51" t="str">
+        <v/>
+      </c>
+      <c r="D51" t="str">
+        <v/>
+      </c>
+      <c r="E51" t="str">
+        <v>323583</v>
+      </c>
+      <c r="F51" t="str">
+        <v>0.00323583</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>DepositManager</v>
+      </c>
+      <c r="B52" t="str">
+        <v>processRequest</v>
+      </c>
+      <c r="C52" t="str">
+        <v/>
+      </c>
+      <c r="D52" t="str">
+        <v/>
+      </c>
+      <c r="E52" t="str">
+        <v>128962</v>
+      </c>
+      <c r="F52" t="str">
+        <v>0.00128962</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>TonContract</v>
+      </c>
+      <c r="B53" t="str">
+        <v>approveAndCall</v>
+      </c>
+      <c r="C53" t="str">
+        <v/>
+      </c>
+      <c r="D53" t="str">
+        <v>DepositManager.onApprove</v>
+      </c>
+      <c r="E53" t="str">
+        <v>322929</v>
+      </c>
+      <c r="F53" t="str">
+        <v>0.00322929</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>DepositManager</v>
+      </c>
+      <c r="B54" t="str">
+        <v>deposit(address,uint256)</v>
+      </c>
+      <c r="C54" t="str">
+        <v/>
+      </c>
+      <c r="D54" t="str">
+        <v/>
+      </c>
+      <c r="E54" t="str">
+        <v>249099</v>
+      </c>
+      <c r="F54" t="str">
+        <v>0.00249099</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>DepositManager</v>
+      </c>
+      <c r="B55" t="str">
+        <v>deposit(address,address,uint256)</v>
+      </c>
+      <c r="C55" t="str">
+        <v/>
+      </c>
+      <c r="D55" t="str">
+        <v/>
+      </c>
+      <c r="E55" t="str">
+        <v>257425</v>
+      </c>
+      <c r="F55" t="str">
+        <v>0.00257425</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>SeigManager</v>
+      </c>
+      <c r="B56" t="str">
+        <v>updateSeigniorageLayer</v>
+      </c>
+      <c r="C56" t="str">
+        <v/>
+      </c>
+      <c r="D56" t="str">
+        <v/>
+      </c>
+      <c r="E56" t="str">
+        <v>354699</v>
+      </c>
+      <c r="F56" t="str">
+        <v>0.00354699</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>DepositManager</v>
+      </c>
+      <c r="B57" t="str">
+        <v>requestWithdrawal</v>
+      </c>
+      <c r="C57" t="str">
+        <v/>
+      </c>
+      <c r="D57" t="str">
+        <v/>
+      </c>
+      <c r="E57" t="str">
+        <v>326832</v>
+      </c>
+      <c r="F57" t="str">
+        <v>0.00326832</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v>DepositManager</v>
+      </c>
+      <c r="B58" t="str">
+        <v>processRequests</v>
+      </c>
+      <c r="C58" t="str">
+        <v/>
+      </c>
+      <c r="D58" t="str">
+        <v/>
+      </c>
+      <c r="E58" t="str">
+        <v>109935</v>
+      </c>
+      <c r="F58" t="str">
+        <v>0.00109935</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F29"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F58"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
refactor: test L1BridgeRegistry changes #35
</commit_message>
<xml_diff>
--- a/outputFile/log-used-gas.xlsx
+++ b/outputFile/log-used-gas.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F58"/>
+  <dimension ref="A1:F60"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -424,7 +424,7 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>L2Registry</v>
+        <v>L1BridgeRegistry</v>
       </c>
       <c r="B2" t="str">
         <v>addManager</v>
@@ -524,7 +524,7 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>L2Registry</v>
+        <v>L1BridgeRegistry</v>
       </c>
       <c r="B7" t="str">
         <v>registerSystemConfigByManager</v>
@@ -536,15 +536,15 @@
         <v/>
       </c>
       <c r="E7" t="str">
-        <v>89648</v>
+        <v>91010</v>
       </c>
       <c r="F7" t="str">
-        <v>0.00089648</v>
+        <v>0.0009101</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>L2Registry</v>
+        <v>L1BridgeRegistry</v>
       </c>
       <c r="B8" t="str">
         <v>setAddresses</v>
@@ -564,7 +564,7 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>L2Registry</v>
+        <v>L1BridgeRegistry</v>
       </c>
       <c r="B9" t="str">
         <v>registerSystemConfigByManager</v>
@@ -576,10 +576,10 @@
         <v xml:space="preserve">Thanos SystemConfig </v>
       </c>
       <c r="E9" t="str">
-        <v>98997</v>
+        <v>100363</v>
       </c>
       <c r="F9" t="str">
-        <v>0.00098997</v>
+        <v>0.00100363</v>
       </c>
     </row>
     <row r="10">
@@ -596,10 +596,10 @@
         <v>using registerLayer2Candidate function</v>
       </c>
       <c r="E10" t="str">
-        <v>4862471</v>
+        <v>4862386</v>
       </c>
       <c r="F10" t="str">
-        <v>0.04862471</v>
+        <v>0.04862386</v>
       </c>
     </row>
     <row r="11">
@@ -696,10 +696,10 @@
         <v>the first updateSeigniorage : no give seigniorage to l2</v>
       </c>
       <c r="E15" t="str">
-        <v>429640</v>
+        <v>429683</v>
       </c>
       <c r="F15" t="str">
-        <v>0.0042964</v>
+        <v>0.00429683</v>
       </c>
     </row>
     <row r="16">
@@ -716,10 +716,10 @@
         <v>the second updateSeigniorage : not operator</v>
       </c>
       <c r="E16" t="str">
-        <v>437487</v>
+        <v>437530</v>
       </c>
       <c r="F16" t="str">
-        <v>0.00437487</v>
+        <v>0.0043753</v>
       </c>
     </row>
     <row r="17">
@@ -736,10 +736,10 @@
         <v>the third updateSeigniorage of operator with claiming</v>
       </c>
       <c r="E17" t="str">
-        <v>480766</v>
+        <v>482606</v>
       </c>
       <c r="F17" t="str">
-        <v>0.00480766</v>
+        <v>0.00482606</v>
       </c>
     </row>
     <row r="18">
@@ -756,10 +756,10 @@
         <v xml:space="preserve">the forth updateSeigniorage of operator with staking </v>
       </c>
       <c r="E18" t="str">
-        <v>588263</v>
+        <v>588145</v>
       </c>
       <c r="F18" t="str">
-        <v>0.00588263</v>
+        <v>0.00588145</v>
       </c>
     </row>
     <row r="19">
@@ -776,10 +776,10 @@
         <v/>
       </c>
       <c r="E19" t="str">
-        <v>341275</v>
+        <v>340683</v>
       </c>
       <c r="F19" t="str">
-        <v>0.00341275</v>
+        <v>0.00340683</v>
       </c>
     </row>
     <row r="20">
@@ -996,15 +996,15 @@
         <v/>
       </c>
       <c r="E30" t="str">
-        <v>476145</v>
+        <v>480828</v>
       </c>
       <c r="F30" t="str">
-        <v>0.00476145</v>
+        <v>0.00480828</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>L2Registry</v>
+        <v>L1BridgeRegistry</v>
       </c>
       <c r="B31" t="str">
         <v>rejectLayer2Candidate</v>
@@ -1024,62 +1024,62 @@
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>L2Registry</v>
+        <v>DepositManager</v>
       </c>
       <c r="B32" t="str">
-        <v>registerLayer2Candidate</v>
+        <v>approveAndCall</v>
       </c>
       <c r="C32" t="str">
         <v/>
       </c>
       <c r="D32" t="str">
-        <v>thanos SystemConfig</v>
+        <v>deposit TON to DAO Candidate</v>
       </c>
       <c r="E32" t="str">
-        <v>4823637</v>
+        <v>340614</v>
       </c>
       <c r="F32" t="str">
-        <v>0.04823637</v>
+        <v>0.00340614</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>SeigManager</v>
+        <v>L1BridgeRegistry</v>
       </c>
       <c r="B33" t="str">
-        <v>updateSeigniorageLayer</v>
+        <v>registerLayer2Candidate</v>
       </c>
       <c r="C33" t="str">
         <v/>
       </c>
       <c r="D33" t="str">
-        <v>titanLayerAddress</v>
+        <v>thanos SystemConfig</v>
       </c>
       <c r="E33" t="str">
-        <v>355902</v>
+        <v>4823495</v>
       </c>
       <c r="F33" t="str">
-        <v>0.00355902</v>
+        <v>0.04823495</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>titanLayerContract</v>
+        <v>SeigManager</v>
       </c>
       <c r="B34" t="str">
-        <v>updateSeigniorage</v>
+        <v>updateSeigniorageLayer</v>
       </c>
       <c r="C34" t="str">
         <v/>
       </c>
       <c r="D34" t="str">
-        <v>with claim</v>
+        <v>titanLayerAddress</v>
       </c>
       <c r="E34" t="str">
-        <v>355815</v>
+        <v>355945</v>
       </c>
       <c r="F34" t="str">
-        <v>0.00355815</v>
+        <v>0.00355945</v>
       </c>
     </row>
     <row r="35">
@@ -1093,93 +1093,93 @@
         <v/>
       </c>
       <c r="D35" t="str">
-        <v>with staking</v>
+        <v>with claim</v>
       </c>
       <c r="E35" t="str">
-        <v>355815</v>
+        <v>355880</v>
       </c>
       <c r="F35" t="str">
-        <v>0.00355815</v>
+        <v>0.0035588</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>DepositManager</v>
+        <v>titanLayerContract</v>
       </c>
       <c r="B36" t="str">
-        <v>deposit(address,uint256)</v>
+        <v>updateSeigniorage</v>
       </c>
       <c r="C36" t="str">
         <v/>
       </c>
       <c r="D36" t="str">
-        <v/>
+        <v>with staking</v>
       </c>
       <c r="E36" t="str">
-        <v>286891</v>
+        <v>355880</v>
       </c>
       <c r="F36" t="str">
-        <v>0.00286891</v>
+        <v>0.0035588</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>SeigManager</v>
+        <v>DepositManager</v>
       </c>
       <c r="B37" t="str">
-        <v>updateSeigniorageLayer</v>
+        <v>deposit(address,uint256)</v>
       </c>
       <c r="C37" t="str">
         <v/>
       </c>
       <c r="D37" t="str">
-        <v>no give seigniorage to l2</v>
+        <v/>
       </c>
       <c r="E37" t="str">
-        <v>435106</v>
+        <v>286891</v>
       </c>
       <c r="F37" t="str">
-        <v>0.00435106</v>
+        <v>0.00286891</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>DepositManager</v>
+        <v>SeigManager</v>
       </c>
       <c r="B38" t="str">
-        <v>deposit(address,address,uint256)</v>
+        <v>updateSeigniorageLayer</v>
       </c>
       <c r="C38" t="str">
         <v/>
       </c>
       <c r="D38" t="str">
-        <v/>
+        <v>no give seigniorage to l2</v>
       </c>
       <c r="E38" t="str">
-        <v>254169</v>
+        <v>435149</v>
       </c>
       <c r="F38" t="str">
-        <v>0.00254169</v>
+        <v>0.00435149</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>SeigManager</v>
+        <v>DepositManager</v>
       </c>
       <c r="B39" t="str">
-        <v>updateSeigniorageLayer</v>
+        <v>deposit(address,address,uint256)</v>
       </c>
       <c r="C39" t="str">
         <v/>
       </c>
       <c r="D39" t="str">
-        <v>give seigniorage to l2</v>
+        <v/>
       </c>
       <c r="E39" t="str">
-        <v>408491</v>
+        <v>254169</v>
       </c>
       <c r="F39" t="str">
-        <v>0.00408491</v>
+        <v>0.00254169</v>
       </c>
     </row>
     <row r="40">
@@ -1193,33 +1193,33 @@
         <v/>
       </c>
       <c r="D40" t="str">
-        <v>not operator</v>
+        <v>give seigniorage to l2</v>
       </c>
       <c r="E40" t="str">
-        <v>408491</v>
+        <v>408534</v>
       </c>
       <c r="F40" t="str">
-        <v>0.00408491</v>
+        <v>0.00408534</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>Layer2Contract</v>
+        <v>SeigManager</v>
       </c>
       <c r="B41" t="str">
-        <v>updateSeigniorage</v>
+        <v>updateSeigniorageLayer</v>
       </c>
       <c r="C41" t="str">
         <v/>
       </c>
       <c r="D41" t="str">
-        <v>operator</v>
+        <v>not operator</v>
       </c>
       <c r="E41" t="str">
-        <v>485970</v>
+        <v>408534</v>
       </c>
       <c r="F41" t="str">
-        <v>0.0048597</v>
+        <v>0.00408534</v>
       </c>
     </row>
     <row r="42">
@@ -1233,33 +1233,33 @@
         <v/>
       </c>
       <c r="D42" t="str">
-        <v>with operator's staking</v>
+        <v>operator</v>
       </c>
       <c r="E42" t="str">
-        <v>593467</v>
+        <v>487810</v>
       </c>
       <c r="F42" t="str">
-        <v>0.00593467</v>
+        <v>0.0048781</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>DepositManager</v>
+        <v>Layer2Contract</v>
       </c>
       <c r="B43" t="str">
-        <v>requestWithdrawal</v>
+        <v>updateSeigniorage</v>
       </c>
       <c r="C43" t="str">
         <v/>
       </c>
       <c r="D43" t="str">
-        <v/>
+        <v>with operator's staking</v>
       </c>
       <c r="E43" t="str">
-        <v>341275</v>
+        <v>593349</v>
       </c>
       <c r="F43" t="str">
-        <v>0.00341275</v>
+        <v>0.00593349</v>
       </c>
     </row>
     <row r="44">
@@ -1267,7 +1267,7 @@
         <v>DepositManager</v>
       </c>
       <c r="B44" t="str">
-        <v>processRequest</v>
+        <v>requestWithdrawal</v>
       </c>
       <c r="C44" t="str">
         <v/>
@@ -1276,18 +1276,18 @@
         <v/>
       </c>
       <c r="E44" t="str">
-        <v>180262</v>
+        <v>341275</v>
       </c>
       <c r="F44" t="str">
-        <v>0.00180262</v>
+        <v>0.00341275</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>L2Registry</v>
+        <v>DepositManager</v>
       </c>
       <c r="B45" t="str">
-        <v>restoreLayer2Candidate</v>
+        <v>processRequest</v>
       </c>
       <c r="C45" t="str">
         <v/>
@@ -1296,18 +1296,18 @@
         <v/>
       </c>
       <c r="E45" t="str">
-        <v>72294</v>
+        <v>180262</v>
       </c>
       <c r="F45" t="str">
-        <v>0.00072294</v>
+        <v>0.00180262</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>SeigManager</v>
+        <v>L1BridgeRegistry</v>
       </c>
       <c r="B46" t="str">
-        <v>updateSeigniorageLayer</v>
+        <v>restoreLayer2Candidate</v>
       </c>
       <c r="C46" t="str">
         <v/>
@@ -1316,10 +1316,10 @@
         <v/>
       </c>
       <c r="E46" t="str">
-        <v>425987</v>
+        <v>72294</v>
       </c>
       <c r="F46" t="str">
-        <v>0.00425987</v>
+        <v>0.00072294</v>
       </c>
     </row>
     <row r="47">
@@ -1336,10 +1336,10 @@
         <v/>
       </c>
       <c r="E47" t="str">
-        <v>403287</v>
+        <v>426030</v>
       </c>
       <c r="F47" t="str">
-        <v>0.00403287</v>
+        <v>0.0042603</v>
       </c>
     </row>
     <row r="48">
@@ -1356,30 +1356,30 @@
         <v/>
       </c>
       <c r="E48" t="str">
-        <v>403287</v>
+        <v>403330</v>
       </c>
       <c r="F48" t="str">
-        <v>0.00403287</v>
+        <v>0.0040333</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>Layer2Contract</v>
+        <v>SeigManager</v>
       </c>
       <c r="B49" t="str">
-        <v>updateSeigniorage</v>
+        <v>updateSeigniorageLayer</v>
       </c>
       <c r="C49" t="str">
         <v/>
       </c>
       <c r="D49" t="str">
-        <v>with operator's claim</v>
+        <v/>
       </c>
       <c r="E49" t="str">
-        <v>463666</v>
+        <v>403330</v>
       </c>
       <c r="F49" t="str">
-        <v>0.00463666</v>
+        <v>0.0040333</v>
       </c>
     </row>
     <row r="50">
@@ -1393,73 +1393,73 @@
         <v/>
       </c>
       <c r="D50" t="str">
-        <v>with operator's staking</v>
+        <v>with operator's claim</v>
       </c>
       <c r="E50" t="str">
-        <v>567880</v>
+        <v>465506</v>
       </c>
       <c r="F50" t="str">
-        <v>0.0056788</v>
+        <v>0.00465506</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>DepositManager</v>
+        <v>Layer2Contract</v>
       </c>
       <c r="B51" t="str">
-        <v>requestWithdrawal</v>
+        <v>updateSeigniorage</v>
       </c>
       <c r="C51" t="str">
         <v/>
       </c>
       <c r="D51" t="str">
-        <v/>
+        <v>with operator's staking</v>
       </c>
       <c r="E51" t="str">
-        <v>323583</v>
+        <v>567828</v>
       </c>
       <c r="F51" t="str">
-        <v>0.00323583</v>
+        <v>0.00567828</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>DepositManager</v>
+        <v>Layer2Contract</v>
       </c>
       <c r="B52" t="str">
-        <v>processRequest</v>
+        <v>updateSeigniorage</v>
       </c>
       <c r="C52" t="str">
         <v/>
       </c>
       <c r="D52" t="str">
-        <v/>
+        <v>with operator's staking</v>
       </c>
       <c r="E52" t="str">
-        <v>128962</v>
+        <v>437710</v>
       </c>
       <c r="F52" t="str">
-        <v>0.00128962</v>
+        <v>0.0043771</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>TonContract</v>
+        <v>DepositManager</v>
       </c>
       <c r="B53" t="str">
-        <v>approveAndCall</v>
+        <v>requestWithdrawal</v>
       </c>
       <c r="C53" t="str">
         <v/>
       </c>
       <c r="D53" t="str">
-        <v>DepositManager.onApprove</v>
+        <v/>
       </c>
       <c r="E53" t="str">
-        <v>322929</v>
+        <v>324175</v>
       </c>
       <c r="F53" t="str">
-        <v>0.00322929</v>
+        <v>0.00324175</v>
       </c>
     </row>
     <row r="54">
@@ -1467,7 +1467,7 @@
         <v>DepositManager</v>
       </c>
       <c r="B54" t="str">
-        <v>deposit(address,uint256)</v>
+        <v>processRequest</v>
       </c>
       <c r="C54" t="str">
         <v/>
@@ -1476,38 +1476,38 @@
         <v/>
       </c>
       <c r="E54" t="str">
-        <v>249099</v>
+        <v>128962</v>
       </c>
       <c r="F54" t="str">
-        <v>0.00249099</v>
+        <v>0.00128962</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>DepositManager</v>
+        <v>TonContract</v>
       </c>
       <c r="B55" t="str">
-        <v>deposit(address,address,uint256)</v>
+        <v>approveAndCall</v>
       </c>
       <c r="C55" t="str">
         <v/>
       </c>
       <c r="D55" t="str">
-        <v/>
+        <v>DepositManager.onApprove</v>
       </c>
       <c r="E55" t="str">
-        <v>257425</v>
+        <v>322929</v>
       </c>
       <c r="F55" t="str">
-        <v>0.00257425</v>
+        <v>0.00322929</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>SeigManager</v>
+        <v>DepositManager</v>
       </c>
       <c r="B56" t="str">
-        <v>updateSeigniorageLayer</v>
+        <v>deposit(address,uint256)</v>
       </c>
       <c r="C56" t="str">
         <v/>
@@ -1516,10 +1516,10 @@
         <v/>
       </c>
       <c r="E56" t="str">
-        <v>354699</v>
+        <v>249099</v>
       </c>
       <c r="F56" t="str">
-        <v>0.00354699</v>
+        <v>0.00249099</v>
       </c>
     </row>
     <row r="57">
@@ -1527,7 +1527,7 @@
         <v>DepositManager</v>
       </c>
       <c r="B57" t="str">
-        <v>requestWithdrawal</v>
+        <v>deposit(address,address,uint256)</v>
       </c>
       <c r="C57" t="str">
         <v/>
@@ -1536,35 +1536,75 @@
         <v/>
       </c>
       <c r="E57" t="str">
-        <v>326832</v>
+        <v>257425</v>
       </c>
       <c r="F57" t="str">
-        <v>0.00326832</v>
+        <v>0.00257425</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
-        <v>DepositManager</v>
+        <v>SeigManager</v>
       </c>
       <c r="B58" t="str">
+        <v>updateSeigniorageLayer</v>
+      </c>
+      <c r="C58" t="str">
+        <v/>
+      </c>
+      <c r="D58" t="str">
+        <v/>
+      </c>
+      <c r="E58" t="str">
+        <v>354699</v>
+      </c>
+      <c r="F58" t="str">
+        <v>0.00354699</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v>DepositManager</v>
+      </c>
+      <c r="B59" t="str">
+        <v>requestWithdrawal</v>
+      </c>
+      <c r="C59" t="str">
+        <v/>
+      </c>
+      <c r="D59" t="str">
+        <v/>
+      </c>
+      <c r="E59" t="str">
+        <v>326832</v>
+      </c>
+      <c r="F59" t="str">
+        <v>0.00326832</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>DepositManager</v>
+      </c>
+      <c r="B60" t="str">
         <v>processRequests</v>
       </c>
-      <c r="C58" t="str">
-        <v/>
-      </c>
-      <c r="D58" t="str">
-        <v/>
-      </c>
-      <c r="E58" t="str">
+      <c r="C60" t="str">
+        <v/>
+      </c>
+      <c r="D60" t="str">
+        <v/>
+      </c>
+      <c r="E60" t="str">
         <v>109935</v>
       </c>
-      <c r="F58" t="str">
+      <c r="F60" t="str">
         <v>0.00109935</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F58"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F60"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>